<commit_message>
reformatted heart rate example files
</commit_message>
<xml_diff>
--- a/example_data/hr_sample_mist.xlsx
+++ b/example_data/hr_sample_mist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Richer/Documents/PhD/Projects/BioPsyKit/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D565E9-A698-CB4C-9A56-43F047BA1F0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CAE15A-C2B7-1C4A-9DD8-C0F8AD8920D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part1" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
   <si>
-    <t>ECG_Rate</t>
+    <t>time</t>
   </si>
   <si>
-    <t>time</t>
+    <t>Heart_Rate</t>
   </si>
 </sst>
 </file>
@@ -439,18 +439,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2395"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -19615,17 +19615,17 @@
   <dimension ref="A1:B810"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -26110,17 +26110,17 @@
   <dimension ref="A1:B737"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -32021,17 +32021,17 @@
   <dimension ref="A1:B684"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -37507,18 +37507,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B3307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>